<commit_message>
Update ER and EDC flow
</commit_message>
<xml_diff>
--- a/TouristApp/Tourist_Design_Schema_rev0.5.xlsx
+++ b/TouristApp/Tourist_Design_Schema_rev0.5.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t xml:space="preserve">This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve">building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenant_id</t>
   </si>
   <si>
     <t xml:space="preserve">tenant_name</t>
@@ -751,10 +754,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -765,14 +768,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="9" width="13"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="9" width="8.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="9" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="9" width="12.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="9" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="9" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="9" width="16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="9" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="9" width="15.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16375" min="16" style="9" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16378" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="9" width="12.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="9" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="9" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="9" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="9" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="9" width="15.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16376" min="17" style="9" width="8.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16379" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -818,17 +821,20 @@
       <c r="N1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="8"/>
+      <c r="O1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="7"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
@@ -837,38 +843,41 @@
         <v>27</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="K2" s="10" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>31</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="7"/>
-      <c r="Q2" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="7"/>
       <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
@@ -876,14 +885,15 @@
       <c r="D3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
-      <c r="Q3" s="8"/>
+      <c r="P3" s="10"/>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
@@ -891,14 +901,15 @@
       <c r="D4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="H4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
-      <c r="Q4" s="8"/>
+      <c r="P4" s="10"/>
+      <c r="R4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
@@ -906,14 +917,15 @@
       <c r="D5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="H5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
-      <c r="Q5" s="8"/>
+      <c r="P5" s="10"/>
+      <c r="R5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10"/>
@@ -921,13 +933,14 @@
       <c r="D6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
@@ -935,13 +948,14 @@
       <c r="D7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="H7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
@@ -949,13 +963,14 @@
       <c r="D8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="H8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10"/>
@@ -963,13 +978,14 @@
       <c r="D9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="H9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
@@ -977,13 +993,14 @@
       <c r="D10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="H10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>